<commit_message>
Web 124 & WEb 125 Updated.\
</commit_message>
<xml_diff>
--- a/124/124.xlsx
+++ b/124/124.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\MFT\004-scores\124\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA093E6A-C00E-40E3-8BE1-3001CFB71854}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{25D31DAE-CACD-4237-ADC5-D75BEA7D980A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="15">
   <si>
     <t>No.</t>
   </si>
@@ -71,6 +71,12 @@
   </si>
   <si>
     <t>H05</t>
+  </si>
+  <si>
+    <t>Q03</t>
+  </si>
+  <si>
+    <t>Q04</t>
   </si>
 </sst>
 </file>
@@ -587,7 +593,7 @@
   <dimension ref="A1:Z37"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+      <selection activeCell="C33" sqref="C33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -628,8 +634,12 @@
       <c r="G1" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="H1" s="2"/>
-      <c r="I1" s="2"/>
+      <c r="H1" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>14</v>
+      </c>
       <c r="J1" s="2"/>
       <c r="K1" s="2"/>
       <c r="L1" s="2"/>
@@ -663,8 +673,14 @@
       <c r="G2" s="4">
         <v>10</v>
       </c>
-      <c r="H2" s="4"/>
-      <c r="I2" s="4"/>
+      <c r="H2" s="4">
+        <f>(19.5/30)*10</f>
+        <v>6.5</v>
+      </c>
+      <c r="I2" s="4">
+        <f>(18/25)*10</f>
+        <v>7.1999999999999993</v>
+      </c>
       <c r="J2" s="4"/>
       <c r="K2" s="4"/>
       <c r="L2" s="4"/>
@@ -707,8 +723,14 @@
       <c r="G3" s="4">
         <v>10.5</v>
       </c>
-      <c r="H3" s="4"/>
-      <c r="I3" s="4"/>
+      <c r="H3" s="4">
+        <f>(15.5/30)*10</f>
+        <v>5.166666666666667</v>
+      </c>
+      <c r="I3" s="4">
+        <f>(13/25)*10</f>
+        <v>5.2</v>
+      </c>
       <c r="J3" s="4"/>
       <c r="K3" s="4"/>
       <c r="L3" s="4"/>
@@ -751,8 +773,14 @@
       <c r="G4" s="4">
         <v>9.5</v>
       </c>
-      <c r="H4" s="4"/>
-      <c r="I4" s="4"/>
+      <c r="H4" s="6">
+        <f>(26.5/30)*10</f>
+        <v>8.8333333333333321</v>
+      </c>
+      <c r="I4" s="4">
+        <f>(14/25)*10</f>
+        <v>5.6000000000000005</v>
+      </c>
       <c r="J4" s="4"/>
       <c r="K4" s="4"/>
       <c r="L4" s="4"/>
@@ -795,8 +823,13 @@
       <c r="G5" s="4">
         <v>9</v>
       </c>
-      <c r="H5" s="4"/>
-      <c r="I5" s="4"/>
+      <c r="H5" s="4">
+        <f>(13/30)*10</f>
+        <v>4.3333333333333339</v>
+      </c>
+      <c r="I5" s="4">
+        <v>0</v>
+      </c>
       <c r="J5" s="4"/>
       <c r="K5" s="4"/>
       <c r="L5" s="4"/>
@@ -839,8 +872,14 @@
       <c r="G6" s="4">
         <v>0</v>
       </c>
-      <c r="H6" s="4"/>
-      <c r="I6" s="4"/>
+      <c r="H6" s="4">
+        <f>(24.5/30)*10</f>
+        <v>8.1666666666666661</v>
+      </c>
+      <c r="I6" s="4">
+        <f>(18/25)*10</f>
+        <v>7.1999999999999993</v>
+      </c>
       <c r="J6" s="4"/>
       <c r="K6" s="4"/>
       <c r="L6" s="4"/>
@@ -883,8 +922,14 @@
       <c r="G7" s="6">
         <v>10</v>
       </c>
-      <c r="H7" s="6"/>
-      <c r="I7" s="6"/>
+      <c r="H7" s="6">
+        <f>(26.5/30)*10</f>
+        <v>8.8333333333333321</v>
+      </c>
+      <c r="I7" s="6">
+        <f>(23/25)*10</f>
+        <v>9.2000000000000011</v>
+      </c>
       <c r="J7" s="6"/>
       <c r="K7" s="6"/>
       <c r="L7" s="6"/>
@@ -927,8 +972,14 @@
       <c r="G8" s="6">
         <v>9.75</v>
       </c>
-      <c r="H8" s="6"/>
-      <c r="I8" s="6"/>
+      <c r="H8" s="6">
+        <f>(23.5/30)*10</f>
+        <v>7.833333333333333</v>
+      </c>
+      <c r="I8" s="6">
+        <f>(24/25)*10</f>
+        <v>9.6</v>
+      </c>
       <c r="J8" s="6"/>
       <c r="K8" s="6"/>
       <c r="L8" s="6"/>
@@ -969,8 +1020,12 @@
       <c r="G9" s="6">
         <v>0</v>
       </c>
-      <c r="H9" s="6"/>
-      <c r="I9" s="6"/>
+      <c r="H9" s="6">
+        <v>0</v>
+      </c>
+      <c r="I9" s="6">
+        <v>0</v>
+      </c>
       <c r="J9" s="6"/>
       <c r="K9" s="6"/>
       <c r="L9" s="6"/>
@@ -1013,8 +1068,13 @@
       <c r="G10" s="6">
         <v>10</v>
       </c>
-      <c r="H10" s="6"/>
-      <c r="I10" s="6"/>
+      <c r="H10" s="6">
+        <f>(29/30)*10</f>
+        <v>9.6666666666666661</v>
+      </c>
+      <c r="I10" s="6">
+        <v>0</v>
+      </c>
       <c r="J10" s="6"/>
       <c r="K10" s="6"/>
       <c r="L10" s="6"/>
@@ -1057,8 +1117,13 @@
       <c r="G11" s="6">
         <v>11</v>
       </c>
-      <c r="H11" s="6"/>
-      <c r="I11" s="6"/>
+      <c r="H11" s="6">
+        <v>0</v>
+      </c>
+      <c r="I11" s="6">
+        <f>(17/25)*10</f>
+        <v>6.8000000000000007</v>
+      </c>
       <c r="J11" s="6"/>
       <c r="K11" s="6"/>
       <c r="L11" s="6"/>
@@ -1101,8 +1166,13 @@
       <c r="G12" s="6">
         <v>10</v>
       </c>
-      <c r="H12" s="6"/>
-      <c r="I12" s="6"/>
+      <c r="H12" s="6">
+        <f>(25/30)*10</f>
+        <v>8.3333333333333339</v>
+      </c>
+      <c r="I12" s="6">
+        <v>0</v>
+      </c>
       <c r="J12" s="6"/>
       <c r="K12" s="6"/>
       <c r="L12" s="6"/>
@@ -1143,8 +1213,12 @@
       <c r="G13" s="6">
         <v>0</v>
       </c>
-      <c r="H13" s="6"/>
-      <c r="I13" s="4"/>
+      <c r="H13" s="6">
+        <v>0</v>
+      </c>
+      <c r="I13" s="4">
+        <v>0</v>
+      </c>
       <c r="J13" s="6"/>
       <c r="K13" s="6"/>
       <c r="L13" s="6"/>
@@ -1253,7 +1327,7 @@
       </c>
       <c r="B17" s="8">
         <f>COUNTA(B1:Q1) * 10</f>
-        <v>60</v>
+        <v>80</v>
       </c>
       <c r="C17" s="5"/>
       <c r="D17" s="5"/>
@@ -1311,21 +1385,21 @@
       </c>
       <c r="B22" s="13">
         <f>(SUM(B2:R2)/B17) * 45</f>
-        <v>37.924999999999997</v>
+        <v>36.15</v>
       </c>
       <c r="C22" s="14">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="D22" s="14">
         <v>0</v>
       </c>
       <c r="E22" s="15">
         <f>B22+C22+D22</f>
-        <v>37.924999999999997</v>
+        <v>44.15</v>
       </c>
       <c r="F22" s="16">
         <f t="shared" ref="F22:F32" si="0">E22</f>
-        <v>37.924999999999997</v>
+        <v>44.15</v>
       </c>
     </row>
     <row r="23" spans="1:26" x14ac:dyDescent="0.25">
@@ -1334,21 +1408,21 @@
       </c>
       <c r="B23" s="13">
         <f>(SUM(B3:R3)/B17) * 45</f>
-        <v>38.5</v>
+        <v>34.706249999999997</v>
       </c>
       <c r="C23" s="14">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="D23" s="14">
         <v>0</v>
       </c>
       <c r="E23" s="15">
         <f t="shared" ref="E23:E32" si="1">B23+C23+D23</f>
-        <v>38.5</v>
+        <v>43.706249999999997</v>
       </c>
       <c r="F23" s="16">
         <f t="shared" si="0"/>
-        <v>38.5</v>
+        <v>43.706249999999997</v>
       </c>
     </row>
     <row r="24" spans="1:26" x14ac:dyDescent="0.25">
@@ -1357,21 +1431,21 @@
       </c>
       <c r="B24" s="13">
         <f>(SUM(B4:R4)/B17) * 45</f>
-        <v>40.749999999999993</v>
+        <v>38.681249999999991</v>
       </c>
       <c r="C24" s="14">
-        <v>0</v>
+        <v>9.5</v>
       </c>
       <c r="D24" s="14">
         <v>0</v>
       </c>
       <c r="E24" s="15">
         <f t="shared" si="1"/>
-        <v>40.749999999999993</v>
+        <v>48.181249999999991</v>
       </c>
       <c r="F24" s="16">
         <f t="shared" si="0"/>
-        <v>40.749999999999993</v>
+        <v>48.181249999999991</v>
       </c>
     </row>
     <row r="25" spans="1:26" x14ac:dyDescent="0.25">
@@ -1380,21 +1454,21 @@
       </c>
       <c r="B25" s="13">
         <f>(SUM(B5:R5)/B17) * 45</f>
-        <v>35.425000000000004</v>
+        <v>29.006250000000001</v>
       </c>
       <c r="C25" s="14">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="D25" s="14">
         <v>0</v>
       </c>
       <c r="E25" s="15">
         <f t="shared" si="1"/>
-        <v>35.425000000000004</v>
+        <v>36.006250000000001</v>
       </c>
       <c r="F25" s="16">
         <f t="shared" si="0"/>
-        <v>35.425000000000004</v>
+        <v>36.006250000000001</v>
       </c>
     </row>
     <row r="26" spans="1:26" x14ac:dyDescent="0.25">
@@ -1403,21 +1477,21 @@
       </c>
       <c r="B26" s="13">
         <f>(SUM(B6:R6)/B17) * 45</f>
-        <v>36.4</v>
+        <v>35.943749999999994</v>
       </c>
       <c r="C26" s="14">
-        <v>0</v>
+        <v>9.5</v>
       </c>
       <c r="D26" s="14">
         <v>0</v>
       </c>
       <c r="E26" s="15">
         <f t="shared" si="1"/>
-        <v>36.4</v>
+        <v>45.443749999999994</v>
       </c>
       <c r="F26" s="16">
         <f t="shared" si="0"/>
-        <v>36.4</v>
+        <v>45.443749999999994</v>
       </c>
     </row>
     <row r="27" spans="1:26" x14ac:dyDescent="0.25">
@@ -1426,21 +1500,21 @@
       </c>
       <c r="B27" s="13">
         <f>(SUM(B7:R7)/B17) * 45</f>
-        <v>41.625</v>
+        <v>41.362500000000004</v>
       </c>
       <c r="C27" s="14">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="D27" s="14">
         <v>0</v>
       </c>
       <c r="E27" s="15">
         <f t="shared" si="1"/>
-        <v>41.625</v>
+        <v>50.362500000000004</v>
       </c>
       <c r="F27" s="16">
         <f t="shared" si="0"/>
-        <v>41.625</v>
+        <v>50.362500000000004</v>
       </c>
     </row>
     <row r="28" spans="1:26" x14ac:dyDescent="0.25">
@@ -1449,21 +1523,21 @@
       </c>
       <c r="B28" s="13">
         <f>(SUM(B8:R8)/B17) * 45</f>
-        <v>42.262500000000003</v>
+        <v>41.503124999999997</v>
       </c>
       <c r="C28" s="14">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="D28" s="14">
         <v>0</v>
       </c>
       <c r="E28" s="15">
         <f t="shared" si="1"/>
-        <v>42.262500000000003</v>
+        <v>50.503124999999997</v>
       </c>
       <c r="F28" s="16">
         <f t="shared" si="0"/>
-        <v>42.262500000000003</v>
+        <v>50.503124999999997</v>
       </c>
     </row>
     <row r="29" spans="1:26" x14ac:dyDescent="0.25">
@@ -1495,21 +1569,21 @@
       </c>
       <c r="B30" s="13">
         <f>(SUM(B10:R10)/B17) * 45</f>
-        <v>37.724999999999994</v>
+        <v>33.731249999999996</v>
       </c>
       <c r="C30" s="14">
-        <v>0</v>
+        <v>7.5</v>
       </c>
       <c r="D30" s="14">
         <v>0</v>
       </c>
       <c r="E30" s="15">
         <f t="shared" si="1"/>
-        <v>37.724999999999994</v>
+        <v>41.231249999999996</v>
       </c>
       <c r="F30" s="16">
         <f t="shared" si="0"/>
-        <v>37.724999999999994</v>
+        <v>41.231249999999996</v>
       </c>
     </row>
     <row r="31" spans="1:26" x14ac:dyDescent="0.25">
@@ -1518,21 +1592,21 @@
       </c>
       <c r="B31" s="13">
         <f>(SUM(B11:R11)/B17) * 45</f>
-        <v>41.2</v>
+        <v>34.725000000000001</v>
       </c>
       <c r="C31" s="14">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="D31" s="14">
         <v>0</v>
       </c>
       <c r="E31" s="15">
         <f t="shared" si="1"/>
-        <v>41.2</v>
+        <v>42.725000000000001</v>
       </c>
       <c r="F31" s="16">
         <f t="shared" si="0"/>
-        <v>41.2</v>
+        <v>42.725000000000001</v>
       </c>
     </row>
     <row r="32" spans="1:26" x14ac:dyDescent="0.25">
@@ -1541,21 +1615,21 @@
       </c>
       <c r="B32" s="13">
         <f>(SUM(B12:R12)/B17) * 45</f>
-        <v>37.475000000000001</v>
+        <v>32.793750000000003</v>
       </c>
       <c r="C32" s="14">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="D32" s="14">
         <v>0</v>
       </c>
       <c r="E32" s="15">
         <f t="shared" si="1"/>
-        <v>37.475000000000001</v>
+        <v>39.793750000000003</v>
       </c>
       <c r="F32" s="16">
         <f t="shared" si="0"/>
-        <v>37.475000000000001</v>
+        <v>39.793750000000003</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.25">
@@ -1605,6 +1679,6 @@
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
-  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Web 124 Homework 06.
</commit_message>
<xml_diff>
--- a/124/124.xlsx
+++ b/124/124.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\MFT\004-scores\124\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{25D31DAE-CACD-4237-ADC5-D75BEA7D980A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{615D4F6C-22C3-42BC-AB46-2D63AB70730D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="16">
   <si>
     <t>No.</t>
   </si>
@@ -77,6 +77,9 @@
   </si>
   <si>
     <t>Q04</t>
+  </si>
+  <si>
+    <t>H06</t>
   </si>
 </sst>
 </file>
@@ -593,7 +596,7 @@
   <dimension ref="A1:Z37"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C33" sqref="C33"/>
+      <selection activeCell="J11" sqref="J11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -640,7 +643,9 @@
       <c r="I1" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="J1" s="2"/>
+      <c r="J1" s="2" t="s">
+        <v>15</v>
+      </c>
       <c r="K1" s="2"/>
       <c r="L1" s="2"/>
       <c r="M1" s="2"/>
@@ -681,7 +686,9 @@
         <f>(18/25)*10</f>
         <v>7.1999999999999993</v>
       </c>
-      <c r="J2" s="4"/>
+      <c r="J2" s="4">
+        <v>9</v>
+      </c>
       <c r="K2" s="4"/>
       <c r="L2" s="4"/>
       <c r="M2" s="4"/>
@@ -731,7 +738,9 @@
         <f>(13/25)*10</f>
         <v>5.2</v>
       </c>
-      <c r="J3" s="4"/>
+      <c r="J3" s="4">
+        <v>9</v>
+      </c>
       <c r="K3" s="4"/>
       <c r="L3" s="4"/>
       <c r="M3" s="4"/>
@@ -781,7 +790,9 @@
         <f>(14/25)*10</f>
         <v>5.6000000000000005</v>
       </c>
-      <c r="J4" s="4"/>
+      <c r="J4" s="4">
+        <v>9</v>
+      </c>
       <c r="K4" s="4"/>
       <c r="L4" s="4"/>
       <c r="M4" s="4"/>
@@ -830,7 +841,9 @@
       <c r="I5" s="4">
         <v>0</v>
       </c>
-      <c r="J5" s="4"/>
+      <c r="J5" s="4">
+        <v>9</v>
+      </c>
       <c r="K5" s="4"/>
       <c r="L5" s="4"/>
       <c r="M5" s="4"/>
@@ -880,7 +893,9 @@
         <f>(18/25)*10</f>
         <v>7.1999999999999993</v>
       </c>
-      <c r="J6" s="4"/>
+      <c r="J6" s="4">
+        <v>0</v>
+      </c>
       <c r="K6" s="4"/>
       <c r="L6" s="4"/>
       <c r="M6" s="4"/>
@@ -930,7 +945,9 @@
         <f>(23/25)*10</f>
         <v>9.2000000000000011</v>
       </c>
-      <c r="J7" s="6"/>
+      <c r="J7" s="6">
+        <v>11</v>
+      </c>
       <c r="K7" s="6"/>
       <c r="L7" s="6"/>
       <c r="M7" s="6"/>
@@ -980,7 +997,9 @@
         <f>(24/25)*10</f>
         <v>9.6</v>
       </c>
-      <c r="J8" s="6"/>
+      <c r="J8" s="6">
+        <v>11</v>
+      </c>
       <c r="K8" s="6"/>
       <c r="L8" s="6"/>
       <c r="M8" s="6"/>
@@ -1026,7 +1045,9 @@
       <c r="I9" s="6">
         <v>0</v>
       </c>
-      <c r="J9" s="6"/>
+      <c r="J9" s="6">
+        <v>0</v>
+      </c>
       <c r="K9" s="6"/>
       <c r="L9" s="6"/>
       <c r="M9" s="6"/>
@@ -1075,7 +1096,9 @@
       <c r="I10" s="6">
         <v>0</v>
       </c>
-      <c r="J10" s="6"/>
+      <c r="J10" s="6">
+        <v>9</v>
+      </c>
       <c r="K10" s="6"/>
       <c r="L10" s="6"/>
       <c r="M10" s="6"/>
@@ -1124,7 +1147,9 @@
         <f>(17/25)*10</f>
         <v>6.8000000000000007</v>
       </c>
-      <c r="J11" s="6"/>
+      <c r="J11" s="6">
+        <v>0</v>
+      </c>
       <c r="K11" s="6"/>
       <c r="L11" s="6"/>
       <c r="M11" s="6"/>
@@ -1173,7 +1198,9 @@
       <c r="I12" s="6">
         <v>0</v>
       </c>
-      <c r="J12" s="6"/>
+      <c r="J12" s="6">
+        <v>8</v>
+      </c>
       <c r="K12" s="6"/>
       <c r="L12" s="6"/>
       <c r="M12" s="6"/>
@@ -1219,7 +1246,9 @@
       <c r="I13" s="4">
         <v>0</v>
       </c>
-      <c r="J13" s="6"/>
+      <c r="J13" s="6">
+        <v>0</v>
+      </c>
       <c r="K13" s="6"/>
       <c r="L13" s="6"/>
       <c r="M13" s="6"/>
@@ -1327,7 +1356,7 @@
       </c>
       <c r="B17" s="8">
         <f>COUNTA(B1:Q1) * 10</f>
-        <v>80</v>
+        <v>90</v>
       </c>
       <c r="C17" s="5"/>
       <c r="D17" s="5"/>
@@ -1385,7 +1414,7 @@
       </c>
       <c r="B22" s="13">
         <f>(SUM(B2:R2)/B17) * 45</f>
-        <v>36.15</v>
+        <v>36.633333333333333</v>
       </c>
       <c r="C22" s="14">
         <v>8</v>
@@ -1395,11 +1424,11 @@
       </c>
       <c r="E22" s="15">
         <f>B22+C22+D22</f>
-        <v>44.15</v>
+        <v>44.633333333333333</v>
       </c>
       <c r="F22" s="16">
         <f t="shared" ref="F22:F32" si="0">E22</f>
-        <v>44.15</v>
+        <v>44.633333333333333</v>
       </c>
     </row>
     <row r="23" spans="1:26" x14ac:dyDescent="0.25">
@@ -1408,7 +1437,7 @@
       </c>
       <c r="B23" s="13">
         <f>(SUM(B3:R3)/B17) * 45</f>
-        <v>34.706249999999997</v>
+        <v>35.349999999999994</v>
       </c>
       <c r="C23" s="14">
         <v>9</v>
@@ -1418,11 +1447,11 @@
       </c>
       <c r="E23" s="15">
         <f t="shared" ref="E23:E32" si="1">B23+C23+D23</f>
-        <v>43.706249999999997</v>
+        <v>44.349999999999994</v>
       </c>
       <c r="F23" s="16">
         <f t="shared" si="0"/>
-        <v>43.706249999999997</v>
+        <v>44.349999999999994</v>
       </c>
     </row>
     <row r="24" spans="1:26" x14ac:dyDescent="0.25">
@@ -1431,7 +1460,7 @@
       </c>
       <c r="B24" s="13">
         <f>(SUM(B4:R4)/B17) * 45</f>
-        <v>38.681249999999991</v>
+        <v>38.883333333333326</v>
       </c>
       <c r="C24" s="14">
         <v>9.5</v>
@@ -1441,11 +1470,11 @@
       </c>
       <c r="E24" s="15">
         <f t="shared" si="1"/>
-        <v>48.181249999999991</v>
+        <v>48.383333333333326</v>
       </c>
       <c r="F24" s="16">
         <f t="shared" si="0"/>
-        <v>48.181249999999991</v>
+        <v>48.383333333333326</v>
       </c>
     </row>
     <row r="25" spans="1:26" x14ac:dyDescent="0.25">
@@ -1454,7 +1483,7 @@
       </c>
       <c r="B25" s="13">
         <f>(SUM(B5:R5)/B17) * 45</f>
-        <v>29.006250000000001</v>
+        <v>30.283333333333335</v>
       </c>
       <c r="C25" s="14">
         <v>7</v>
@@ -1464,11 +1493,11 @@
       </c>
       <c r="E25" s="15">
         <f t="shared" si="1"/>
-        <v>36.006250000000001</v>
+        <v>37.283333333333331</v>
       </c>
       <c r="F25" s="16">
         <f t="shared" si="0"/>
-        <v>36.006250000000001</v>
+        <v>37.283333333333331</v>
       </c>
     </row>
     <row r="26" spans="1:26" x14ac:dyDescent="0.25">
@@ -1477,7 +1506,7 @@
       </c>
       <c r="B26" s="13">
         <f>(SUM(B6:R6)/B17) * 45</f>
-        <v>35.943749999999994</v>
+        <v>31.949999999999992</v>
       </c>
       <c r="C26" s="14">
         <v>9.5</v>
@@ -1487,11 +1516,11 @@
       </c>
       <c r="E26" s="15">
         <f t="shared" si="1"/>
-        <v>45.443749999999994</v>
+        <v>41.449999999999989</v>
       </c>
       <c r="F26" s="16">
         <f t="shared" si="0"/>
-        <v>45.443749999999994</v>
+        <v>41.449999999999989</v>
       </c>
     </row>
     <row r="27" spans="1:26" x14ac:dyDescent="0.25">
@@ -1500,7 +1529,7 @@
       </c>
       <c r="B27" s="13">
         <f>(SUM(B7:R7)/B17) * 45</f>
-        <v>41.362500000000004</v>
+        <v>42.266666666666666</v>
       </c>
       <c r="C27" s="14">
         <v>9</v>
@@ -1510,11 +1539,11 @@
       </c>
       <c r="E27" s="15">
         <f t="shared" si="1"/>
-        <v>50.362500000000004</v>
+        <v>51.266666666666666</v>
       </c>
       <c r="F27" s="16">
         <f t="shared" si="0"/>
-        <v>50.362500000000004</v>
+        <v>51.266666666666666</v>
       </c>
     </row>
     <row r="28" spans="1:26" x14ac:dyDescent="0.25">
@@ -1523,7 +1552,7 @@
       </c>
       <c r="B28" s="13">
         <f>(SUM(B8:R8)/B17) * 45</f>
-        <v>41.503124999999997</v>
+        <v>42.391666666666666</v>
       </c>
       <c r="C28" s="14">
         <v>9</v>
@@ -1533,11 +1562,11 @@
       </c>
       <c r="E28" s="15">
         <f t="shared" si="1"/>
-        <v>50.503124999999997</v>
+        <v>51.391666666666666</v>
       </c>
       <c r="F28" s="16">
         <f t="shared" si="0"/>
-        <v>50.503124999999997</v>
+        <v>51.391666666666666</v>
       </c>
     </row>
     <row r="29" spans="1:26" x14ac:dyDescent="0.25">
@@ -1569,7 +1598,7 @@
       </c>
       <c r="B30" s="13">
         <f>(SUM(B10:R10)/B17) * 45</f>
-        <v>33.731249999999996</v>
+        <v>34.483333333333334</v>
       </c>
       <c r="C30" s="14">
         <v>7.5</v>
@@ -1579,11 +1608,11 @@
       </c>
       <c r="E30" s="15">
         <f t="shared" si="1"/>
-        <v>41.231249999999996</v>
+        <v>41.983333333333334</v>
       </c>
       <c r="F30" s="16">
         <f t="shared" si="0"/>
-        <v>41.231249999999996</v>
+        <v>41.983333333333334</v>
       </c>
     </row>
     <row r="31" spans="1:26" x14ac:dyDescent="0.25">
@@ -1592,7 +1621,7 @@
       </c>
       <c r="B31" s="13">
         <f>(SUM(B11:R11)/B17) * 45</f>
-        <v>34.725000000000001</v>
+        <v>30.866666666666667</v>
       </c>
       <c r="C31" s="14">
         <v>8</v>
@@ -1602,11 +1631,11 @@
       </c>
       <c r="E31" s="15">
         <f t="shared" si="1"/>
-        <v>42.725000000000001</v>
+        <v>38.866666666666667</v>
       </c>
       <c r="F31" s="16">
         <f t="shared" si="0"/>
-        <v>42.725000000000001</v>
+        <v>38.866666666666667</v>
       </c>
     </row>
     <row r="32" spans="1:26" x14ac:dyDescent="0.25">
@@ -1615,7 +1644,7 @@
       </c>
       <c r="B32" s="13">
         <f>(SUM(B12:R12)/B17) * 45</f>
-        <v>32.793750000000003</v>
+        <v>33.150000000000006</v>
       </c>
       <c r="C32" s="14">
         <v>7</v>
@@ -1625,11 +1654,11 @@
       </c>
       <c r="E32" s="15">
         <f t="shared" si="1"/>
-        <v>39.793750000000003</v>
+        <v>40.150000000000006</v>
       </c>
       <c r="F32" s="16">
         <f t="shared" si="0"/>
-        <v>39.793750000000003</v>
+        <v>40.150000000000006</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.25">

</xml_diff>